<commit_message>
add excel test cases
</commit_message>
<xml_diff>
--- a/Assets/TC_List.xlsx
+++ b/Assets/TC_List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tegpam/Katalon Studio/OrangeHRM-Katalon/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5682BC1A-07BA-5541-9DE4-187041E2C9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4722C6-B41F-6E4F-B03F-1F6ECD2EB1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{3A1534E2-CFF9-BF4E-9318-7B651ECBFC74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{3A1534E2-CFF9-BF4E-9318-7B651ECBFC74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -167,6 +168,42 @@
   <si>
     <t>username: Admin 
 password: blank fields</t>
+  </si>
+  <si>
+    <t>TC_LogWorkIn_001</t>
+  </si>
+  <si>
+    <t>User Loged Work (in)</t>
+  </si>
+  <si>
+    <t>Logged Work</t>
+  </si>
+  <si>
+    <t>User on dashboard page</t>
+  </si>
+  <si>
+    <t>Success alert pop up</t>
+  </si>
+  <si>
+    <t>On Progress</t>
+  </si>
+  <si>
+    <t>1. Click Menu "Time"</t>
+  </si>
+  <si>
+    <t>2. Click Top Bar "Attendance"</t>
+  </si>
+  <si>
+    <t>3. Click Punch In/Out</t>
+  </si>
+  <si>
+    <t>4. Select Desired Date</t>
+  </si>
+  <si>
+    <t>5. Select Desired Time</t>
+  </si>
+  <si>
+    <t>6. Click In</t>
   </si>
 </sst>
 </file>
@@ -210,12 +247,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43F0961-4FBA-0D42-9E47-615459BC1287}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,24 +885,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="A5:A7"/>
@@ -879,6 +901,183 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="I8:I10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E59A0B-977D-AA4E-8CAB-C598DB3FD9C1}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="I2:I7"/>
+    <mergeCell ref="J2:J7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="H2:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>